<commit_message>
MAJOR CHANGES. Originally started out making and adding the AccountTreeListView, but then it exploded into a lot more changes. Add the Queries.cs file to keep track of the information that is only read from the database (view type information). The major part of these Queries was to gather the information for the AccountTreeListView. Added the AccountCatagory table into the design so to make selecting an Accounts catagory (Account, Income, expense) easy. Also added the AEBalance table to keep track of its balances. Also added the endingBalance and currentBalance back into the Envelope and Account tables. Added static functions in the FFDBDataSet to recalculate the ending and starting balances of the Envelope, Account, and AEBalance tables.
</commit_message>
<xml_diff>
--- a/Design/Project Design.xlsx
+++ b/Design/Project Design.xlsx
@@ -7540,13 +7540,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>544284</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>394606</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>-1</xdr:rowOff>
@@ -7650,13 +7650,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>421820</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>272142</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>149679</xdr:rowOff>
@@ -7790,13 +7790,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>521153</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>68036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>137431</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>68035</xdr:rowOff>
@@ -7918,13 +7918,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>5041</xdr:rowOff>
@@ -8016,13 +8016,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -8183,19 +8183,49 @@
             <a:t>envelopes</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>currentBalance</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>endingBalance</a:t>
+          </a:r>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>398318</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>16080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>520782</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>16082</xdr:rowOff>
@@ -8369,13 +8399,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>547996</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>16082</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>166996</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>16081</xdr:rowOff>
@@ -8519,13 +8549,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>166996</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>109228</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>398318</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>109228</xdr:rowOff>
@@ -8564,14 +8594,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8582,8 +8612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="493059" y="627530"/>
-          <a:ext cx="1692088" cy="1411941"/>
+          <a:off x="495300" y="571501"/>
+          <a:ext cx="1695450" cy="1457324"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -8692,9 +8722,7 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
+          <a:pPr rtl="0"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
               <a:solidFill>
@@ -8705,6 +8733,64 @@
             </a:rPr>
             <a:t>closed</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>currentBalance</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>endingBalance</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8712,13 +8798,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>2521</xdr:rowOff>
@@ -8755,141 +8841,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>134471</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>11207</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>11205</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>11206</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6220" name="AutoShape 76"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="13828059" y="324972"/>
-          <a:ext cx="1086970" cy="941293"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartAlternateProcess">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="sng" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>AEBalance</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>id</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>accountID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>envelopeID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>endingBalance</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -8981,13 +8939,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -9402,13 +9360,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>503464</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>367393</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
@@ -9530,13 +9488,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>54428</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>81643</xdr:rowOff>
@@ -9658,13 +9616,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>277090</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>103909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>138545</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>103909</xdr:rowOff>
@@ -9763,13 +9721,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>299355</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>27214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>323848</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>27214</xdr:rowOff>
@@ -10033,13 +9991,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>259773</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>69273</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>502227</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>69273</xdr:rowOff>
@@ -10153,13 +10111,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>1589</xdr:rowOff>
@@ -10196,14 +10154,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>839647</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>708819</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>794</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>841235</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>710407</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>795</xdr:rowOff>
     </xdr:to>
@@ -10218,8 +10176,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="3507441" y="2431677"/>
-          <a:ext cx="470648" cy="1588"/>
+          <a:off x="4772025" y="2509838"/>
+          <a:ext cx="485776" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10240,13 +10198,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>846044</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>700089</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>840441</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>709614</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -10261,8 +10219,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="2227169" y="1151405"/>
-          <a:ext cx="627530" cy="2403662"/>
+          <a:off x="2743201" y="481013"/>
+          <a:ext cx="723901" cy="3819525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10285,13 +10243,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>1589</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10304,8 +10262,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2185147" y="3922059"/>
-          <a:ext cx="2409265" cy="1"/>
+          <a:off x="2190750" y="4048126"/>
+          <a:ext cx="3076575" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10326,13 +10284,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>845251</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>794</xdr:rowOff>
+      <xdr:colOff>699295</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>86519</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>846839</xdr:colOff>
+      <xdr:colOff>700883</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>795</xdr:rowOff>
     </xdr:to>
@@ -10347,8 +10305,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="711574" y="2667001"/>
-          <a:ext cx="1255059" cy="1588"/>
+          <a:off x="509588" y="2714626"/>
+          <a:ext cx="1371601" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10368,13 +10326,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>686921</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>7844</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>12885</xdr:rowOff>
@@ -10466,13 +10424,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>10365</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>686921</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -10490,6 +10448,264 @@
         <a:xfrm flipV="1">
           <a:off x="4591050" y="658065"/>
           <a:ext cx="686921" cy="637335"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="AutoShape 73"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2857500" y="571500"/>
+          <a:ext cx="1695450" cy="1457324"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="sng" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>AEBalance</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>accountID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>envelopeID</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>currentBalance</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr rtl="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>endingBalance</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="AutoShape 93"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks noChangeShapeType="1"/>
+          <a:stCxn id="29" idx="1"/>
+          <a:endCxn id="6217" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="2190750" y="1300161"/>
+          <a:ext cx="666750" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="AutoShape 93"/>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks noChangeShapeType="1"/>
+          <a:stCxn id="29" idx="3"/>
+          <a:endCxn id="6211" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipV="1">
+          <a:off x="4552950" y="1295400"/>
+          <a:ext cx="523875" cy="4762"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -12716,58 +12932,70 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A11:I71"/>
+  <dimension ref="A11:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="21" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" s="35"/>
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" s="35"/>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" s="35"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
       <c r="D16" s="35"/>
       <c r="E16" s="35"/>
       <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:6">
       <c r="A22" s="35"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:6">
       <c r="A28" s="35"/>
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:11">
       <c r="A36" s="35"/>
       <c r="B36" s="35"/>
       <c r="C36" s="35"/>
@@ -12777,21 +13005,29 @@
       <c r="G36" s="35"/>
       <c r="H36" s="35"/>
       <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:11">
       <c r="A42" s="35"/>
       <c r="B42" s="35"/>
       <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:5">
       <c r="A51" s="35"/>
       <c r="B51" s="35"/>
       <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="35"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:5">
       <c r="A71" s="35"/>
       <c r="B71" s="35"/>
       <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -12799,7 +13035,7 @@
   <pageSetup scale="89" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="4" max="1048575" man="1"/>
+    <brk id="6" max="1048575" man="1"/>
   </colBreaks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Made lots of changes. Removed ALL dependent columns (LineItem.oppAccountID, LineItem.envelopeID). Also added the Testing Folder with the stressTest class. Currently stress test simulates about 100 years of data to all the tables: ~100k transactions, 258k line items, 830 accounts.
</commit_message>
<xml_diff>
--- a/Design/Project Design.xlsx
+++ b/Design/Project Design.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Design Key</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>N  - Not Tested</t>
+  </si>
+  <si>
+    <t>Views</t>
   </si>
 </sst>
 </file>
@@ -7918,16 +7921,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>5041</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>14566</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7938,8 +7941,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5286375" y="1457325"/>
-          <a:ext cx="1171575" cy="652741"/>
+          <a:off x="6657975" y="1304925"/>
+          <a:ext cx="1371600" cy="652741"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -8018,7 +8021,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -8036,8 +8039,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2902324" y="313765"/>
-          <a:ext cx="1680882" cy="1882588"/>
+          <a:off x="4552950" y="971550"/>
+          <a:ext cx="1419225" cy="1295400"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -8120,7 +8123,7 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>accountTypeID</a:t>
+            <a:t>typeID</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -8135,7 +8138,7 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>categoryID</a:t>
+            <a:t>category</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -8181,36 +8184,6 @@
               <a:cs typeface="Arial"/>
             </a:rPr>
             <a:t>envelopes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>currentBalance</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>endingBalance</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8592,13 +8565,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -8612,8 +8585,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="495300" y="571501"/>
-          <a:ext cx="1695450" cy="1457324"/>
+          <a:off x="2486025" y="885825"/>
+          <a:ext cx="1400175" cy="1143000"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -8696,22 +8669,7 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>fullName</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>parentEnvelope</a:t>
+            <a:t>groupID</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
             <a:solidFill>
@@ -8742,56 +8700,6 @@
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
         </a:p>
-        <a:p>
-          <a:pPr rtl="0"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>currentBalance</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr rtl="0"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>endingBalance</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -8800,14 +8708,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>2521</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12046</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8820,8 +8728,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4591050" y="1295400"/>
-          <a:ext cx="695325" cy="488296"/>
+          <a:off x="5972175" y="1619250"/>
+          <a:ext cx="685800" cy="12046"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8842,15 +8750,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8861,8 +8769,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7126941" y="3608295"/>
-          <a:ext cx="1277471" cy="627529"/>
+          <a:off x="6686550" y="3505201"/>
+          <a:ext cx="1371600" cy="647699"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -8947,8 +8855,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8959,8 +8867,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4594412" y="2667001"/>
-          <a:ext cx="1680882" cy="2510117"/>
+          <a:off x="4552950" y="2752726"/>
+          <a:ext cx="1419225" cy="2152649"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -9083,12 +8991,12 @@
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>oppAccountID</a:t>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>description</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -9103,7 +9011,7 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>description</a:t>
+            <a:t>confermationNumber</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -9118,7 +9026,7 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>confermationNumber</a:t>
+            <a:t>complete</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -9128,12 +9036,12 @@
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>envelopeID</a:t>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>amount</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -9148,68 +9056,15 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>complete</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>amount</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
             <a:t>creditDebit</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>transactionError</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>lineError</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -9217,16 +9072,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9237,8 +9092,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="493059" y="3294530"/>
-          <a:ext cx="1692088" cy="1255058"/>
+          <a:off x="2476500" y="3181351"/>
+          <a:ext cx="1400175" cy="1295399"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -9269,7 +9124,7 @@
               <a:latin typeface="Arial"/>
               <a:cs typeface="Arial"/>
             </a:rPr>
-            <a:t>SubLineItem</a:t>
+            <a:t>EnvelopeLine</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
             <a:solidFill>
@@ -10113,14 +9968,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1589</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106364</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10133,8 +9988,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6275294" y="3922060"/>
-          <a:ext cx="851647" cy="1588"/>
+          <a:off x="5972175" y="3829051"/>
+          <a:ext cx="714375" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10176,7 +10031,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="4772025" y="2509838"/>
+          <a:off x="5019675" y="2509838"/>
           <a:ext cx="485776" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -10197,59 +10052,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>700089</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>709614</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29775" name="AutoShape 93"/>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks noChangeShapeType="1"/>
-          <a:stCxn id="6224" idx="0"/>
-          <a:endCxn id="6217" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm rot="16200000" flipV="1">
-          <a:off x="2743201" y="481013"/>
-          <a:ext cx="723901" cy="3819525"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>1589</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106364</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10262,8 +10074,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2190750" y="4048126"/>
-          <a:ext cx="3076575" cy="1588"/>
+          <a:off x="3876675" y="3829051"/>
+          <a:ext cx="676275" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10283,16 +10095,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>699295</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>690562</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>86519</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>700883</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>795</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>700087</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104777</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10305,8 +10117,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="509588" y="2714626"/>
-          <a:ext cx="1371601" cy="1588"/>
+          <a:off x="2605087" y="2600326"/>
+          <a:ext cx="1152526" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10326,157 +10138,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>686921</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7844</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12885</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="AutoShape 66"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5277971" y="331694"/>
-          <a:ext cx="1380004" cy="652741"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartAlternateProcess">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="sng" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>AccountCatagory</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>id</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>name</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>10365</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>686921</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="AutoShape 74"/>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks noChangeShapeType="1"/>
-          <a:stCxn id="6211" idx="3"/>
-          <a:endCxn id="26" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="4591050" y="658065"/>
-          <a:ext cx="686921" cy="637335"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -10487,8 +10158,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2857500" y="571500"/>
-          <a:ext cx="1695450" cy="1457324"/>
+          <a:off x="8877300" y="1466850"/>
+          <a:ext cx="1219200" cy="1457324"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -10603,25 +10274,6 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:pPr rtl="0"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>endingBalance</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
           <a:pPr algn="l" rtl="0">
             <a:defRPr sz="1000"/>
           </a:pPr>
@@ -10639,73 +10291,128 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>5041</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="AutoShape 66"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="628650" y="1133475"/>
+          <a:ext cx="1371600" cy="652741"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="0" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="sng" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>EnvelopeGroup</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial"/>
+            <a:cs typeface="Arial"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>name</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="AutoShape 93"/>
+        <xdr:cNvPr id="36" name="AutoShape 97"/>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks noChangeShapeType="1"/>
-          <a:stCxn id="29" idx="1"/>
-          <a:endCxn id="6217" idx="3"/>
+          <a:stCxn id="6217" idx="1"/>
+          <a:endCxn id="28" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="2190750" y="1300161"/>
-          <a:ext cx="666750" cy="1"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="AutoShape 93"/>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks noChangeShapeType="1"/>
-          <a:stCxn id="29" idx="3"/>
-          <a:endCxn id="6211" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm flipV="1">
-          <a:off x="4552950" y="1295400"/>
-          <a:ext cx="523875" cy="4762"/>
+          <a:off x="2000251" y="1457324"/>
+          <a:ext cx="485775" cy="2521"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -12932,47 +12639,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A11:K71"/>
+  <dimension ref="C7:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="20.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10" style="4" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" style="4" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="4" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="4" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="11" spans="1:8">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
+    <row r="7" spans="3:10">
+      <c r="J7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>
       <c r="F11" s="35"/>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
+    <row r="13" spans="3:10">
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
       <c r="E13" s="35"/>
       <c r="F13" s="35"/>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+    <row r="16" spans="3:10">
       <c r="C16" s="35"/>
       <c r="D16" s="35"/>
       <c r="E16" s="35"/>
@@ -12980,24 +12686,18 @@
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="35"/>
-      <c r="B22" s="35"/>
+    <row r="22" spans="3:6">
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
       <c r="E22" s="35"/>
       <c r="F22" s="35"/>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="35"/>
-      <c r="B28" s="35"/>
+    <row r="28" spans="3:6">
       <c r="C28" s="35"/>
       <c r="D28" s="35"/>
       <c r="E28" s="35"/>
     </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="35"/>
-      <c r="B36" s="35"/>
+    <row r="36" spans="3:11">
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
       <c r="E36" s="35"/>
@@ -13008,23 +12708,17 @@
       <c r="J36" s="35"/>
       <c r="K36" s="35"/>
     </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="35"/>
-      <c r="B42" s="35"/>
+    <row r="42" spans="3:11">
       <c r="C42" s="35"/>
       <c r="D42" s="35"/>
       <c r="E42" s="35"/>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="35"/>
-      <c r="B51" s="35"/>
+    <row r="51" spans="3:5">
       <c r="C51" s="35"/>
       <c r="D51" s="35"/>
       <c r="E51" s="35"/>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="35"/>
-      <c r="B71" s="35"/>
+    <row r="71" spans="3:5">
       <c r="C71" s="35"/>
       <c r="D71" s="35"/>
       <c r="E71" s="35"/>

</xml_diff>